<commit_message>
Fix Excel formulas for Cyclophosphamide, Taxane
</commit_message>
<xml_diff>
--- a/StudyDocuments/NCI Secondary Malignancies_Abstraction MSW.xlsx
+++ b/StudyDocuments/NCI Secondary Malignancies_Abstraction MSW.xlsx
@@ -12832,50 +12832,7 @@
     <cellStyle name="Normal 3" xfId="3"/>
     <cellStyle name="Normal 4" xfId="1"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -13183,7 +13140,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13378,11 +13335,11 @@
         <v>1</v>
       </c>
       <c r="U3" s="16" t="b">
-        <f>OR(ISNUMBER(SEARCH("cyclophosphamide", F3)), ISNUMBER(SEARCH("cytoxan", F3)))</f>
-        <v>0</v>
+        <f>OR(ISNUMBER(SEARCH("cyclophosph?mide", E3)), ISNUMBER(SEARCH("cytoxan", E3)))</f>
+        <v>1</v>
       </c>
       <c r="V3" s="16" t="b">
-        <f>OR(ISNUMBER(SEARCH("taxane", G3)), ISNUMBER(SEARCH("paclitaxel", G3)), ISNUMBER(SEARCH("docetaxel", G3)))</f>
+        <f>OR(ISNUMBER(SEARCH("taxane", E3)), ISNUMBER(SEARCH("paclitaxel", E3)), ISNUMBER(SEARCH("docetaxel", E3)))</f>
         <v>0</v>
       </c>
     </row>
@@ -13437,11 +13394,11 @@
         <v>1</v>
       </c>
       <c r="U4" s="16" t="b">
-        <f t="shared" ref="U4:U20" si="1">OR(ISNUMBER(SEARCH("cyclophosphamide", F4)), ISNUMBER(SEARCH("cytoxan", F4)))</f>
-        <v>0</v>
+        <f t="shared" ref="U4:U20" si="1">OR(ISNUMBER(SEARCH("cyclophosph?mide", E4)), ISNUMBER(SEARCH("cytoxan", E4)))</f>
+        <v>1</v>
       </c>
       <c r="V4" s="16" t="b">
-        <f t="shared" ref="V4:V20" si="2">OR(ISNUMBER(SEARCH("taxane", G4)), ISNUMBER(SEARCH("paclitaxel", G4)), ISNUMBER(SEARCH("docetaxel", G4)))</f>
+        <f t="shared" ref="V4:V20" si="2">OR(ISNUMBER(SEARCH("taxane", E4)), ISNUMBER(SEARCH("paclitaxel", E4)), ISNUMBER(SEARCH("docetaxel", E4)))</f>
         <v>0</v>
       </c>
     </row>
@@ -13554,7 +13511,7 @@
       </c>
       <c r="U6" s="16" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V6" s="16" t="b">
         <f t="shared" si="2"/>
@@ -13611,7 +13568,7 @@
       </c>
       <c r="U7" s="16" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V7" s="16" t="b">
         <f t="shared" si="2"/>
@@ -13668,7 +13625,7 @@
       </c>
       <c r="U8" s="16" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V8" s="16" t="b">
         <f t="shared" si="2"/>
@@ -13841,7 +13798,7 @@
       </c>
       <c r="U11" s="16" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V11" s="16" t="b">
         <f t="shared" si="2"/>
@@ -13902,7 +13859,7 @@
       </c>
       <c r="V12" s="16" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="384" x14ac:dyDescent="0.2">

</xml_diff>